<commit_message>
Update with stats from penultimate game 10/21/15
Luke hit for the cycle
</commit_message>
<xml_diff>
--- a/Minor League Scientists Stats.xlsx
+++ b/Minor League Scientists Stats.xlsx
@@ -71,27 +71,30 @@
     <t>Oliver Patton</t>
   </si>
   <si>
+    <t>Rich Squitieri</t>
+  </si>
+  <si>
     <t>Qaiser Patel</t>
   </si>
   <si>
+    <t>Luke Heuer</t>
+  </si>
+  <si>
     <t>Nick Mirman</t>
   </si>
   <si>
     <t>Joe Edwards</t>
   </si>
   <si>
-    <t>Rich Squitieri</t>
-  </si>
-  <si>
     <t>Zac Chestnut</t>
   </si>
   <si>
+    <t>Derek Bayes</t>
+  </si>
+  <si>
     <t>Charlie Henschen</t>
   </si>
   <si>
-    <t>Luke Heuer</t>
-  </si>
-  <si>
     <t>Amory Meltzer</t>
   </si>
   <si>
@@ -99,9 +102,6 @@
   </si>
   <si>
     <t>Scott Richardson</t>
-  </si>
-  <si>
-    <t>Derek Bayes</t>
   </si>
   <si>
     <t>Total:</t>
@@ -475,7 +475,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="str">
         <f>4+3+4
@@ -538,7 +538,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" ref="B6:C6" si="8">3+3+4</f>
@@ -598,7 +598,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" ref="B7:C7" si="10">3+3+3</f>
@@ -657,7 +657,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" ref="B8:C8" si="11">3+3+3</f>
@@ -717,7 +717,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" ref="B9:C9" si="12">4+3+3</f>
@@ -777,7 +777,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" ref="B10:B11" si="15">3+3+3</f>
@@ -839,7 +839,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" si="15"/>
@@ -900,7 +900,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="str">
         <f t="shared" ref="B12:C12" si="16">1</f>
@@ -1111,26 +1111,26 @@
         <v>16</v>
       </c>
       <c r="B2" s="3" t="str">
-        <f>4+4+3+5+3</f>
-        <v>19</v>
+        <f>4+4+3+5+3+5</f>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f>4+2+3+5+3</f>
+        <f>4+2+3+5+3+5</f>
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f>3+3+2+3+2+4</f>
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="str">
-        <f>3+3+2+3+2</f>
-        <v>13</v>
-      </c>
       <c r="E2" s="3" t="str">
-        <f>4+2+2+4+2</f>
-        <v>14</v>
+        <f>4+2+2+4+2+4</f>
+        <v>18</v>
       </c>
       <c r="F2" s="3">
         <v>2.0</v>
       </c>
       <c r="G2" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H2" s="3" t="str">
         <f>1+1
@@ -1138,9 +1138,9 @@
         <v>2</v>
       </c>
       <c r="I2" s="3" t="str">
-        <f>3+4+5
-</f>
-        <v>12</v>
+        <f>3+4+5+3
+</f>
+        <v>15</v>
       </c>
       <c r="J2" s="3">
         <v>2.0</v>
@@ -1154,19 +1154,19 @@
       <c r="M2" s="4"/>
       <c r="N2" s="5" t="str">
         <f t="shared" ref="N2:N17" si="1">IF(C2,E2/C2,)</f>
-        <v>0.824</v>
+        <v>0.818</v>
       </c>
       <c r="O2" s="5" t="str">
         <f t="shared" ref="O2:O17" si="2">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
-        <v>1.294</v>
+        <v>1.273</v>
       </c>
       <c r="P2" s="5" t="str">
         <f t="shared" ref="P2:P18" si="3">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
-        <v>0.842</v>
+        <v>0.833</v>
       </c>
       <c r="Q2" s="5" t="str">
         <f t="shared" ref="Q2:Q18" si="4">IF(O2,O2+P2,)</f>
-        <v>2.136</v>
+        <v>2.106</v>
       </c>
     </row>
     <row r="3">
@@ -1174,20 +1174,20 @@
         <v>18</v>
       </c>
       <c r="B3" s="3" t="str">
-        <f>4+4+3+4+3</f>
-        <v>18</v>
+        <f>4+4+3+4+3+5</f>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f>4+4+3+3+2</f>
-        <v>16</v>
+        <f>4+4+3+3+2+5</f>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>3+3+1+1</f>
-        <v>8</v>
+        <f>3+3+1+1+2</f>
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>3+3+1+2</f>
-        <v>9</v>
+        <f>3+3+1+2+4</f>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="str">
         <f>2+1
@@ -1195,15 +1195,15 @@
         <v>3</v>
       </c>
       <c r="G3" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H3" s="3" t="str">
         <f>0+2</f>
         <v>2</v>
       </c>
       <c r="I3" s="3" t="str">
-        <f>2+4+2</f>
-        <v>8</v>
+        <f>2+4+2+3</f>
+        <v>11</v>
       </c>
       <c r="J3" s="3" t="str">
         <f>1
@@ -1219,55 +1219,55 @@
       <c r="M3" s="4"/>
       <c r="N3" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.563</v>
+        <v>0.619</v>
       </c>
       <c r="O3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.125</v>
+        <v>1.143</v>
       </c>
       <c r="P3" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.556</v>
+        <v>0.609</v>
       </c>
       <c r="Q3" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.681</v>
+        <v>1.752</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="str">
-        <f t="shared" ref="B4:C4" si="5">4+3+3+4+2</f>
-        <v>16</v>
+        <f t="shared" ref="B4:C4" si="5">4+3+3+4+2+5</f>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>2+1
-</f>
-        <v>3</v>
+        <f>2+1+1
+</f>
+        <v>4</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>9+2+1
-</f>
-        <v>12</v>
+        <f>9+2+1+2
+</f>
+        <v>14</v>
       </c>
       <c r="F4" s="3">
         <v>2.0</v>
       </c>
       <c r="G4" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H4" s="3">
         <v>0.0</v>
       </c>
       <c r="I4" s="3" t="str">
-        <f>3+1+3+1</f>
-        <v>8</v>
+        <f>3+1+3+1+3</f>
+        <v>11</v>
       </c>
       <c r="J4" s="3">
         <v>0.0</v>
@@ -1281,58 +1281,60 @@
       <c r="M4" s="4"/>
       <c r="N4" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.750</v>
+        <v>0.667</v>
       </c>
       <c r="O4" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.875</v>
+        <v>0.857</v>
       </c>
       <c r="P4" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.750</v>
+        <v>0.667</v>
       </c>
       <c r="Q4" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.625</v>
+        <v>1.524</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="str">
-        <f>4+3+4+3</f>
-        <v>14</v>
+        <f>4+3+4+3+5</f>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="str">
-        <f>4+3+3+3
+        <f>4+3+3+3+5
+</f>
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>1+1+3+3</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="str">
+        <f>3+2+3+4
+</f>
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f>1+1
+</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="str">
+        <f>3+1
+</f>
+        <v>4</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I5" s="3" t="str">
+        <f>5+4+4
 </f>
         <v>13</v>
-      </c>
-      <c r="D5" s="3" t="str">
-        <f>1+1+3</f>
-        <v>5</v>
-      </c>
-      <c r="E5" s="3" t="str">
-        <f>3+2+3
-</f>
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="str">
-        <f>1
-</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="3" t="str">
-        <f>5+4
-</f>
-        <v>9</v>
       </c>
       <c r="J5" s="3">
         <v>0.0</v>
@@ -1346,24 +1348,24 @@
       <c r="M5" s="4"/>
       <c r="N5" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.615</v>
+        <v>0.667</v>
       </c>
       <c r="O5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.154</v>
+        <v>1.389</v>
       </c>
       <c r="P5" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.571</v>
+        <v>0.632</v>
       </c>
       <c r="Q5" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.725</v>
+        <v>2.020</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="str">
         <f>4+3+3
@@ -1426,33 +1428,35 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="str">
-        <f t="shared" ref="B7:C7" si="6">4+3+4+3</f>
-        <v>14</v>
+        <f>4+3+4+3+5</f>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v>14</v>
+        <f>4+3+4+3+4</f>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>1+3+1
-</f>
-        <v>5</v>
+        <f>1+3+1+1
+</f>
+        <v>6</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>3+2+3+2
-</f>
-        <v>10</v>
+        <f>3+2+3+2+3
+</f>
+        <v>13</v>
       </c>
       <c r="F7" s="3" t="str">
         <f>1+2
 </f>
         <v>3</v>
       </c>
-      <c r="G7" s="3">
-        <v>1.0</v>
+      <c r="G7" s="3" t="str">
+        <f>1+1
+</f>
+        <v>2</v>
       </c>
       <c r="H7" s="3" t="str">
         <f>1
@@ -1460,8 +1464,8 @@
         <v>1</v>
       </c>
       <c r="I7" s="3" t="str">
-        <f>1+1+2+1</f>
-        <v>5</v>
+        <f>1+1+2+1+2</f>
+        <v>7</v>
       </c>
       <c r="J7" s="3">
         <v>0.0</v>
@@ -1469,30 +1473,32 @@
       <c r="K7" s="3">
         <v>0.0</v>
       </c>
-      <c r="L7" s="3">
-        <v>0.0</v>
+      <c r="L7" s="3" t="str">
+        <f>1
+</f>
+        <v>1</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.714</v>
+        <v>0.722</v>
       </c>
       <c r="O7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.286</v>
+        <v>1.278</v>
       </c>
       <c r="P7" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.714</v>
+        <v>0.684</v>
       </c>
       <c r="Q7" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>2.000</v>
+        <v>1.962</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="str">
         <f>3+4+2
@@ -1560,20 +1566,20 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="str">
-        <f t="shared" ref="B9:C9" si="7">4+4+3+2</f>
-        <v>13</v>
+        <f t="shared" ref="B9:C9" si="6">4+4+3+2+5</f>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>13</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="str">
         <f>1+2+1+1</f>
         <v>5</v>
       </c>
       <c r="E9" s="3" t="str">
-        <f>2+2+2+1</f>
-        <v>7</v>
+        <f>2+2+2+1+2</f>
+        <v>9</v>
       </c>
       <c r="F9" s="3">
         <v>0.0</v>
@@ -1585,8 +1591,8 @@
         <v>0.0</v>
       </c>
       <c r="I9" s="3" t="str">
-        <f>1+1+1</f>
-        <v>3</v>
+        <f>1+1+1+1</f>
+        <v>4</v>
       </c>
       <c r="J9" s="3">
         <v>0.0</v>
@@ -1600,41 +1606,41 @@
       <c r="M9" s="4"/>
       <c r="N9" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.538</v>
+        <v>0.500</v>
       </c>
       <c r="O9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.538</v>
+        <v>0.500</v>
       </c>
       <c r="P9" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.538</v>
+        <v>0.500</v>
       </c>
       <c r="Q9" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.077</v>
+        <v>1.000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="str">
-        <f t="shared" ref="B10:C10" si="8">3+3+3+4</f>
-        <v>13</v>
+        <f t="shared" ref="B10:C10" si="7">3+3+3+4+4</f>
+        <v>17</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>13</v>
+        <f t="shared" si="7"/>
+        <v>17</v>
       </c>
       <c r="D10" s="3" t="str">
-        <f>1+2
-</f>
-        <v>3</v>
+        <f>1+2+3
+</f>
+        <v>6</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f>1+1+1+3</f>
-        <v>6</v>
+        <f>1+1+1+3+3</f>
+        <v>9</v>
       </c>
       <c r="F10" s="3">
         <v>1.0</v>
@@ -1642,12 +1648,14 @@
       <c r="G10" s="3">
         <v>0.0</v>
       </c>
-      <c r="H10" s="3">
-        <v>0.0</v>
+      <c r="H10" s="3" t="str">
+        <f>1
+</f>
+        <v>1</v>
       </c>
       <c r="I10" s="3" t="str">
-        <f>1+1+2</f>
-        <v>4</v>
+        <f>1+1+2+1</f>
+        <v>5</v>
       </c>
       <c r="J10" s="3">
         <v>0.0</v>
@@ -1661,31 +1669,31 @@
       <c r="M10" s="4"/>
       <c r="N10" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.462</v>
+        <v>0.529</v>
       </c>
       <c r="O10" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.538</v>
+        <v>0.765</v>
       </c>
       <c r="P10" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.462</v>
+        <v>0.529</v>
       </c>
       <c r="Q10" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.000</v>
+        <v>1.294</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="str">
-        <f t="shared" ref="B11:C11" si="9">3+3+3+4+2</f>
+        <f t="shared" ref="B11:C11" si="8">3+3+3+4+2</f>
         <v>15</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D11" s="3" t="str">
@@ -1741,23 +1749,23 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3" t="str">
-        <f t="shared" ref="B12:B13" si="10">3+3+3+4+2</f>
-        <v>15</v>
+        <f t="shared" ref="B12:B13" si="9">3+3+3+4+2+4</f>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f t="shared" ref="C12:C13" si="11">3+3+3+4+1</f>
-        <v>14</v>
+        <f>3+3+3+4+1+3</f>
+        <v>17</v>
       </c>
       <c r="D12" s="3" t="str">
-        <f>1+1+3+2</f>
-        <v>7</v>
+        <f>1+1+3+2+3</f>
+        <v>10</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f>1+2+1+3</f>
-        <v>7</v>
+        <f>1+2+1+3+2</f>
+        <v>9</v>
       </c>
       <c r="F12" s="3">
         <v>0.0</v>
@@ -1769,14 +1777,14 @@
         <v>0.0</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f>1+3
-</f>
-        <v>4</v>
+        <f>1+3+1
+</f>
+        <v>5</v>
       </c>
       <c r="J12" s="3" t="str">
-        <f t="shared" ref="J12:J13" si="12">1
-</f>
-        <v>1</v>
+        <f>1+1
+</f>
+        <v>2</v>
       </c>
       <c r="K12" s="3">
         <v>0.0</v>
@@ -1787,44 +1795,44 @@
       <c r="M12" s="4"/>
       <c r="N12" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.500</v>
+        <v>0.529</v>
       </c>
       <c r="O12" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.500</v>
+        <v>0.529</v>
       </c>
       <c r="P12" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.533</v>
+        <v>0.579</v>
       </c>
       <c r="Q12" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.033</v>
+        <v>1.108</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>15</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>14</v>
+        <f>3+3+3+4+1+4</f>
+        <v>18</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f>2+1+3+2
-</f>
-        <v>8</v>
+        <f>2+1+3+2+1
+</f>
+        <v>9</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f>2+2+1+3</f>
-        <v>8</v>
+        <f>2+2+1+3+2</f>
+        <v>10</v>
       </c>
       <c r="F13" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G13" s="3">
         <v>0.0</v>
@@ -1833,12 +1841,13 @@
         <v>0.0</v>
       </c>
       <c r="I13" s="3" t="str">
-        <f>2+3
-</f>
-        <v>5</v>
+        <f>2+3+1
+</f>
+        <v>6</v>
       </c>
       <c r="J13" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f>1
+</f>
         <v>1</v>
       </c>
       <c r="K13" s="3">
@@ -1850,19 +1859,19 @@
       <c r="M13" s="4"/>
       <c r="N13" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.571</v>
+        <v>0.556</v>
       </c>
       <c r="O13" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.571</v>
+        <v>0.611</v>
       </c>
       <c r="P13" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.600</v>
+        <v>0.579</v>
       </c>
       <c r="Q13" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.171</v>
+        <v>1.190</v>
       </c>
     </row>
     <row r="14">
@@ -1870,12 +1879,12 @@
         <v>31</v>
       </c>
       <c r="B14" s="3" t="str">
-        <f t="shared" ref="B14:C14" si="13">3+4
+        <f t="shared" ref="B14:C14" si="10">3+4
 </f>
         <v>7</v>
       </c>
       <c r="C14" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="D14" s="3">
@@ -1927,28 +1936,29 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3" t="str">
-        <f>4+3</f>
+        <f>4+3+5</f>
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f>4+1+4</f>
+        <v>9</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f>2+3
+</f>
+        <v>5</v>
+      </c>
+      <c r="E15" s="3" t="str">
+        <f>3+1+3</f>
         <v>7</v>
       </c>
-      <c r="C15" s="3" t="str">
-        <f>4+1</f>
-        <v>5</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f>2</f>
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="str">
-        <f>3+1</f>
-        <v>4</v>
-      </c>
       <c r="F15" s="3" t="str">
-        <f>1
-</f>
-        <v>1</v>
+        <f>1+1
+</f>
+        <v>2</v>
       </c>
       <c r="G15" s="3">
         <v>0.0</v>
@@ -1957,8 +1967,8 @@
         <v>0.0</v>
       </c>
       <c r="I15" s="3" t="str">
-        <f>3+2</f>
-        <v>5</v>
+        <f>3+2+2</f>
+        <v>7</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>2</f>
@@ -1967,13 +1977,15 @@
       <c r="K15" s="3">
         <v>0.0</v>
       </c>
-      <c r="L15" s="3">
-        <v>0.0</v>
+      <c r="L15" s="3" t="str">
+        <f>1
+</f>
+        <v>1</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.800</v>
+        <v>0.778</v>
       </c>
       <c r="O15" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1981,11 +1993,11 @@
       </c>
       <c r="P15" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.857</v>
+        <v>0.750</v>
       </c>
       <c r="Q15" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.857</v>
+        <v>1.750</v>
       </c>
     </row>
     <row r="16">
@@ -2103,65 +2115,65 @@
         <v>30</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f t="shared" ref="B18:L18" si="14">sum(B2:B17)</f>
-        <v>192</v>
+        <f t="shared" ref="B18:L18" si="11">sum(B2:B17)</f>
+        <v>239</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v>180</v>
+        <f t="shared" si="11"/>
+        <v>224</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v>80</v>
+        <f t="shared" si="11"/>
+        <v>101</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v>112</v>
+        <f t="shared" si="11"/>
+        <v>141</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v>17</v>
+        <f t="shared" si="11"/>
+        <v>20</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v>5</v>
+        <f t="shared" si="11"/>
+        <v>10</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v>5</v>
+        <f t="shared" si="11"/>
+        <v>7</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v>80</v>
+        <f t="shared" si="11"/>
+        <v>101</v>
       </c>
       <c r="J18" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v>10</v>
+        <f t="shared" si="11"/>
+        <v>11</v>
       </c>
       <c r="K18" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="L18" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f t="shared" si="11"/>
+        <v>4</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="6" t="str">
         <f>E18/C18</f>
-        <v>0.622</v>
+        <v>0.629</v>
       </c>
       <c r="O18" s="6" t="str">
         <f>((E18-F18-G18-H18)+(2*F18)+(3*G18)+(4*H18))/C18</f>
-        <v>0.856</v>
+        <v>0.902</v>
       </c>
       <c r="P18" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>0.635</v>
+        <v>0.636</v>
       </c>
       <c r="Q18" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>1.491</v>
+        <v>1.538</v>
       </c>
     </row>
     <row r="22">

</xml_diff>

<commit_message>
More closely match lineup
</commit_message>
<xml_diff>
--- a/Minor League Scientists Stats.xlsx
+++ b/Minor League Scientists Stats.xlsx
@@ -71,40 +71,40 @@
     <t>Oliver Patton</t>
   </si>
   <si>
+    <t>Qaiser Patel</t>
+  </si>
+  <si>
+    <t>Nick Mirman</t>
+  </si>
+  <si>
+    <t>Joe Edwards</t>
+  </si>
+  <si>
+    <t>Luke Heuer</t>
+  </si>
+  <si>
+    <t>Zac Chestnut</t>
+  </si>
+  <si>
+    <t>Charlie Henschen</t>
+  </si>
+  <si>
+    <t>Amory Meltzer</t>
+  </si>
+  <si>
+    <t>Derek Bayes</t>
+  </si>
+  <si>
+    <t>Gordon Walker</t>
+  </si>
+  <si>
+    <t>Scott Richardson</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
     <t>Rich Squitieri</t>
-  </si>
-  <si>
-    <t>Qaiser Patel</t>
-  </si>
-  <si>
-    <t>Luke Heuer</t>
-  </si>
-  <si>
-    <t>Nick Mirman</t>
-  </si>
-  <si>
-    <t>Joe Edwards</t>
-  </si>
-  <si>
-    <t>Zac Chestnut</t>
-  </si>
-  <si>
-    <t>Derek Bayes</t>
-  </si>
-  <si>
-    <t>Charlie Henschen</t>
-  </si>
-  <si>
-    <t>Amory Meltzer</t>
-  </si>
-  <si>
-    <t>Gordon Walker</t>
-  </si>
-  <si>
-    <t>Scott Richardson</t>
-  </si>
-  <si>
-    <t>Total:</t>
   </si>
   <si>
     <t>Andrew Scott</t>
@@ -475,7 +475,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="str">
         <f>4+3+4
@@ -538,7 +538,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" ref="B6:C6" si="8">3+3+4</f>
@@ -598,7 +598,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" ref="B7:C7" si="10">3+3+3</f>
@@ -657,7 +657,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" ref="B8:C8" si="11">3+3+3</f>
@@ -717,7 +717,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" ref="B9:C9" si="12">4+3+3</f>
@@ -777,7 +777,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" ref="B10:B11" si="15">3+3+3</f>
@@ -839,7 +839,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" si="15"/>
@@ -900,7 +900,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3" t="str">
         <f t="shared" ref="B12:C12" si="16">1</f>
@@ -959,7 +959,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" ref="B13:L13" si="18">sum(B2:B12)</f>
@@ -1239,66 +1239,69 @@
         <v>19</v>
       </c>
       <c r="B4" s="3" t="str">
-        <f t="shared" ref="B4:C4" si="5">4+3+3+4+2+5</f>
-        <v>21</v>
+        <f>4+3+5</f>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>21</v>
+        <f>4+1+4</f>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>2+1+1
-</f>
-        <v>4</v>
+        <f>2+3</f>
+        <v>5</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>9+2+1+2
-</f>
-        <v>14</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2.0</v>
+        <f>3+1+3</f>
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f t="shared" ref="F4:F5" si="5">1+1
+</f>
+        <v>2</v>
       </c>
       <c r="G4" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H4" s="3">
         <v>0.0</v>
       </c>
       <c r="I4" s="3" t="str">
-        <f>3+1+3+1+3</f>
-        <v>11</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.0</v>
+        <f>3+2+2</f>
+        <v>7</v>
+      </c>
+      <c r="J4" s="3" t="str">
+        <f>2</f>
+        <v>2</v>
       </c>
       <c r="K4" s="3">
         <v>0.0</v>
       </c>
-      <c r="L4" s="3">
-        <v>0.0</v>
+      <c r="L4" s="3" t="str">
+        <f>1
+</f>
+        <v>1</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.667</v>
+        <v>0.778</v>
       </c>
       <c r="O4" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.857</v>
+        <v>1.000</v>
       </c>
       <c r="P4" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.667</v>
+        <v>0.750</v>
       </c>
       <c r="Q4" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.524</v>
+        <v>1.750</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="str">
         <f>4+3+4+3+5</f>
@@ -1319,8 +1322,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>1+1
-</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G5" s="3" t="str">
@@ -1365,7 +1367,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="str">
         <f>4+3+3
@@ -1428,7 +1430,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="str">
         <f>4+3+4+3+5</f>
@@ -1498,44 +1500,41 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="str">
-        <f>3+4+2
-</f>
-        <v>9</v>
+        <f t="shared" ref="B8:C8" si="6">4+3+3+4+2+5</f>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="str">
-        <f>3+4+1
-</f>
-        <v>8</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3.0</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>2+1+1
+</f>
+        <v>4</v>
       </c>
       <c r="E8" s="3" t="str">
-        <f>2+3
-</f>
-        <v>5</v>
+        <f>9+2+1+2
+</f>
+        <v>14</v>
       </c>
       <c r="F8" s="3">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G8" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H8" s="3">
         <v>0.0</v>
       </c>
       <c r="I8" s="3" t="str">
-        <f>2+2
-</f>
-        <v>4</v>
-      </c>
-      <c r="J8" s="3" t="str">
-        <f>1
-</f>
-        <v>1</v>
+        <f>3+1+3+1+3</f>
+        <v>11</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.0</v>
       </c>
       <c r="K8" s="3">
         <v>0.0</v>
@@ -1546,11 +1545,11 @@
       <c r="M8" s="4"/>
       <c r="N8" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>0.667</v>
       </c>
       <c r="O8" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.625</v>
+        <v>0.857</v>
       </c>
       <c r="P8" s="5" t="str">
         <f t="shared" si="3"/>
@@ -1558,105 +1557,106 @@
       </c>
       <c r="Q8" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.292</v>
+        <v>1.524</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f>3+4+2
+</f>
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f>3+4+1
+</f>
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E9" s="3" t="str">
+        <f>2+3</f>
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I9" s="3" t="str">
+        <f>2+2
+</f>
+        <v>4</v>
+      </c>
+      <c r="J9" s="3" t="str">
+        <f>1
+</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+      <c r="O9" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>0.625</v>
+      </c>
+      <c r="P9" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.667</v>
+      </c>
+      <c r="Q9" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>1.292</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="str">
-        <f t="shared" ref="B9:C9" si="6">4+4+3+2+5</f>
+      <c r="B10" s="3" t="str">
+        <f t="shared" ref="B10:C10" si="7">4+4+3+2+5</f>
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C10" s="3" t="str">
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="D9" s="3" t="str">
+      <c r="D10" s="3" t="str">
         <f>1+2+1+1</f>
         <v>5</v>
       </c>
-      <c r="E9" s="3" t="str">
+      <c r="E10" s="3" t="str">
         <f>2+2+2+1+2</f>
         <v>9</v>
       </c>
-      <c r="F9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I9" s="3" t="str">
+      <c r="F10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I10" s="3" t="str">
         <f>1+1+1+1</f>
         <v>4</v>
       </c>
-      <c r="J9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.500</v>
-      </c>
-      <c r="O9" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.500</v>
-      </c>
-      <c r="P9" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.500</v>
-      </c>
-      <c r="Q9" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="3" t="str">
-        <f t="shared" ref="B10:C10" si="7">3+3+3+4+4</f>
-        <v>17</v>
-      </c>
-      <c r="C10" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>17</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f>1+2+3
-</f>
-        <v>6</v>
-      </c>
-      <c r="E10" s="3" t="str">
-        <f>1+1+1+3+3</f>
-        <v>9</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H10" s="3" t="str">
-        <f>1
-</f>
-        <v>1</v>
-      </c>
-      <c r="I10" s="3" t="str">
-        <f>1+1+2+1</f>
-        <v>5</v>
-      </c>
       <c r="J10" s="3">
         <v>0.0</v>
       </c>
@@ -1669,24 +1669,24 @@
       <c r="M10" s="4"/>
       <c r="N10" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.529</v>
+        <v>0.500</v>
       </c>
       <c r="O10" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.765</v>
+        <v>0.500</v>
       </c>
       <c r="P10" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.529</v>
+        <v>0.500</v>
       </c>
       <c r="Q10" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.294</v>
+        <v>1.000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" ref="B11:C11" si="8">3+3+3+4+2</f>
@@ -1752,39 +1752,39 @@
         <v>28</v>
       </c>
       <c r="B12" s="3" t="str">
-        <f t="shared" ref="B12:B13" si="9">3+3+3+4+2+4</f>
-        <v>19</v>
+        <f t="shared" ref="B12:C12" si="9">3+3+3+4+4</f>
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f>3+3+3+4+1+3</f>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="D12" s="3" t="str">
-        <f>1+1+3+2+3</f>
-        <v>10</v>
+        <f>1+2+3
+</f>
+        <v>6</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f>1+2+1+3+2</f>
+        <f>1+1+1+3+3</f>
         <v>9</v>
       </c>
       <c r="F12" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G12" s="3">
         <v>0.0</v>
       </c>
-      <c r="H12" s="3">
-        <v>0.0</v>
+      <c r="H12" s="3" t="str">
+        <f>1
+</f>
+        <v>1</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f>1+3+1
-</f>
+        <f>1+1+2+1</f>
         <v>5</v>
       </c>
-      <c r="J12" s="3" t="str">
-        <f>1+1
-</f>
-        <v>2</v>
+      <c r="J12" s="3">
+        <v>0.0</v>
       </c>
       <c r="K12" s="3">
         <v>0.0</v>
@@ -1799,23 +1799,23 @@
       </c>
       <c r="O12" s="5" t="str">
         <f t="shared" si="2"/>
+        <v>0.765</v>
+      </c>
+      <c r="P12" s="5" t="str">
+        <f t="shared" si="3"/>
         <v>0.529</v>
       </c>
-      <c r="P12" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.579</v>
-      </c>
       <c r="Q12" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.108</v>
+        <v>1.294</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="B13:B14" si="10">3+3+3+4+2+4</f>
         <v>19</v>
       </c>
       <c r="C13" s="3" t="str">
@@ -1876,24 +1876,23 @@
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="str">
-        <f t="shared" ref="B14:C14" si="10">3+4
-</f>
-        <v>7</v>
+        <f t="shared" si="10"/>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3.0</v>
+        <f>3+3+3+4+1+3</f>
+        <v>17</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f>1+1+3+2+3</f>
+        <v>10</v>
       </c>
       <c r="E14" s="3" t="str">
-        <f>1+3
-</f>
-        <v>4</v>
+        <f>1+2+1+3+2</f>
+        <v>9</v>
       </c>
       <c r="F14" s="3">
         <v>0.0</v>
@@ -1904,11 +1903,15 @@
       <c r="H14" s="3">
         <v>0.0</v>
       </c>
-      <c r="I14" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0.0</v>
+      <c r="I14" s="3" t="str">
+        <f>1+3+1
+</f>
+        <v>5</v>
+      </c>
+      <c r="J14" s="3" t="str">
+        <f>1+1
+</f>
+        <v>2</v>
       </c>
       <c r="K14" s="3">
         <v>0.0</v>
@@ -1919,46 +1922,44 @@
       <c r="M14" s="4"/>
       <c r="N14" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.571</v>
+        <v>0.529</v>
       </c>
       <c r="O14" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.571</v>
+        <v>0.529</v>
       </c>
       <c r="P14" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.571</v>
+        <v>0.579</v>
       </c>
       <c r="Q14" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.143</v>
+        <v>1.108</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="str">
-        <f>4+3+5</f>
-        <v>12</v>
+        <f t="shared" ref="B15:C15" si="11">3+4
+</f>
+        <v>7</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f>4+1+4</f>
-        <v>9</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f>2+3
-</f>
-        <v>5</v>
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3.0</v>
       </c>
       <c r="E15" s="3" t="str">
-        <f>3+1+3</f>
-        <v>7</v>
-      </c>
-      <c r="F15" s="3" t="str">
-        <f>1+1
-</f>
-        <v>2</v>
+        <f>1+3
+</f>
+        <v>4</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.0</v>
       </c>
       <c r="G15" s="3">
         <v>0.0</v>
@@ -1966,38 +1967,34 @@
       <c r="H15" s="3">
         <v>0.0</v>
       </c>
-      <c r="I15" s="3" t="str">
-        <f>3+2+2</f>
-        <v>7</v>
-      </c>
-      <c r="J15" s="3" t="str">
-        <f>2</f>
-        <v>2</v>
+      <c r="I15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.0</v>
       </c>
       <c r="K15" s="3">
         <v>0.0</v>
       </c>
-      <c r="L15" s="3" t="str">
-        <f>1
-</f>
-        <v>1</v>
+      <c r="L15" s="3">
+        <v>0.0</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>0.778</v>
+        <v>0.571</v>
       </c>
       <c r="O15" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.000</v>
+        <v>0.571</v>
       </c>
       <c r="P15" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0.750</v>
+        <v>0.571</v>
       </c>
       <c r="Q15" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>1.750</v>
+        <v>1.143</v>
       </c>
     </row>
     <row r="16">
@@ -2112,50 +2109,50 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f t="shared" ref="B18:L18" si="11">sum(B2:B17)</f>
+        <f t="shared" ref="B18:L18" si="12">sum(B2:B17)</f>
         <v>239</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>224</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>101</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>141</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>101</v>
       </c>
       <c r="J18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="K18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="L18" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="M18" s="3"/>

</xml_diff>

<commit_message>
Update with data from 10/28/15 game
Last game of the season :(
</commit_message>
<xml_diff>
--- a/Minor League Scientists Stats.xlsx
+++ b/Minor League Scientists Stats.xlsx
@@ -98,13 +98,13 @@
     <t>Gordon Walker</t>
   </si>
   <si>
+    <t>Rich Squitieri</t>
+  </si>
+  <si>
     <t>Scott Richardson</t>
   </si>
   <si>
     <t>Total:</t>
-  </si>
-  <si>
-    <t>Rich Squitieri</t>
   </si>
   <si>
     <t>Andrew Scott</t>
@@ -184,6 +184,9 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
@@ -191,9 +194,6 @@
       <alignment/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -330,20 +330,20 @@
       <c r="L2" s="3">
         <v>0.0</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5" t="str">
+      <c r="M2" s="5"/>
+      <c r="N2" s="6" t="str">
         <f t="shared" ref="N2:N13" si="1">IF(C2,E2/C2,)</f>
         <v>0.700</v>
       </c>
-      <c r="O2" s="5" t="str">
+      <c r="O2" s="6" t="str">
         <f t="shared" ref="O2:O13" si="2">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
         <v>0.727</v>
       </c>
-      <c r="P2" s="5" t="str">
+      <c r="P2" s="6" t="str">
         <f t="shared" ref="P2:P13" si="3">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
         <v>1.000</v>
       </c>
-      <c r="Q2" s="5" t="str">
+      <c r="Q2" s="6" t="str">
         <f t="shared" ref="Q2:Q13" si="4">IF(P2,P2+O2,)</f>
         <v>1.727</v>
       </c>
@@ -391,20 +391,20 @@
       <c r="L3" s="3">
         <v>0.0</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="5" t="str">
+      <c r="M3" s="5"/>
+      <c r="N3" s="6" t="str">
         <f t="shared" si="1"/>
         <v>0.625</v>
       </c>
-      <c r="O3" s="5" t="str">
+      <c r="O3" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0.700</v>
       </c>
-      <c r="P3" s="5" t="str">
+      <c r="P3" s="6" t="str">
         <f t="shared" si="3"/>
         <v>0.625</v>
       </c>
-      <c r="Q3" s="5" t="str">
+      <c r="Q3" s="6" t="str">
         <f t="shared" si="4"/>
         <v>1.325</v>
       </c>
@@ -455,20 +455,20 @@
       <c r="L4" s="3">
         <v>0.0</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="5" t="str">
+      <c r="M4" s="5"/>
+      <c r="N4" s="6" t="str">
         <f t="shared" si="1"/>
         <v>0.778</v>
       </c>
-      <c r="O4" s="5" t="str">
+      <c r="O4" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0.778</v>
       </c>
-      <c r="P4" s="5" t="str">
+      <c r="P4" s="6" t="str">
         <f t="shared" si="3"/>
         <v>1.222</v>
       </c>
-      <c r="Q4" s="5" t="str">
+      <c r="Q4" s="6" t="str">
         <f t="shared" si="4"/>
         <v>2.000</v>
       </c>
@@ -518,20 +518,20 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="5" t="str">
+      <c r="M5" s="5"/>
+      <c r="N5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>0.400</v>
       </c>
-      <c r="O5" s="5" t="str">
+      <c r="O5" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0.364</v>
       </c>
-      <c r="P5" s="5" t="str">
+      <c r="P5" s="6" t="str">
         <f t="shared" si="3"/>
         <v>0.500</v>
       </c>
-      <c r="Q5" s="5" t="str">
+      <c r="Q5" s="6" t="str">
         <f t="shared" si="4"/>
         <v>0.864</v>
       </c>
@@ -578,20 +578,20 @@
       <c r="L6" s="3">
         <v>0.0</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="5" t="str">
+      <c r="M6" s="5"/>
+      <c r="N6" s="6" t="str">
         <f t="shared" si="1"/>
         <v>0.400</v>
       </c>
-      <c r="O6" s="5" t="str">
+      <c r="O6" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0.400</v>
       </c>
-      <c r="P6" s="5" t="str">
+      <c r="P6" s="6" t="str">
         <f t="shared" si="3"/>
         <v>0.400</v>
       </c>
-      <c r="Q6" s="5" t="str">
+      <c r="Q6" s="6" t="str">
         <f t="shared" si="4"/>
         <v>0.800</v>
       </c>
@@ -637,20 +637,20 @@
       <c r="L7" s="3">
         <v>0.0</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="5" t="str">
+      <c r="M7" s="5"/>
+      <c r="N7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>0.333</v>
       </c>
-      <c r="O7" s="5" t="str">
+      <c r="O7" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0.333</v>
       </c>
-      <c r="P7" s="5" t="str">
+      <c r="P7" s="6" t="str">
         <f t="shared" si="3"/>
         <v>0.333</v>
       </c>
-      <c r="Q7" s="5" t="str">
+      <c r="Q7" s="6" t="str">
         <f t="shared" si="4"/>
         <v>0.667</v>
       </c>
@@ -697,20 +697,20 @@
       <c r="L8" s="3">
         <v>0.0</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="5" t="str">
+      <c r="M8" s="5"/>
+      <c r="N8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>0.667</v>
       </c>
-      <c r="O8" s="5" t="str">
+      <c r="O8" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0.667</v>
       </c>
-      <c r="P8" s="5" t="str">
+      <c r="P8" s="6" t="str">
         <f t="shared" si="3"/>
         <v>0.667</v>
       </c>
-      <c r="Q8" s="5" t="str">
+      <c r="Q8" s="6" t="str">
         <f t="shared" si="4"/>
         <v>1.333</v>
       </c>
@@ -757,20 +757,20 @@
       <c r="L9" s="3">
         <v>0.0</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="5" t="str">
+      <c r="M9" s="5"/>
+      <c r="N9" s="6" t="str">
         <f t="shared" si="1"/>
         <v>0.600</v>
       </c>
-      <c r="O9" s="5" t="str">
+      <c r="O9" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0.600</v>
       </c>
-      <c r="P9" s="5" t="str">
+      <c r="P9" s="6" t="str">
         <f t="shared" si="3"/>
         <v>0.800</v>
       </c>
-      <c r="Q9" s="5" t="str">
+      <c r="Q9" s="6" t="str">
         <f t="shared" si="4"/>
         <v>1.400</v>
       </c>
@@ -819,20 +819,20 @@
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="5" t="str">
+      <c r="M10" s="5"/>
+      <c r="N10" s="6" t="str">
         <f t="shared" si="1"/>
         <v>0.571</v>
       </c>
-      <c r="O10" s="5" t="str">
+      <c r="O10" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0.444</v>
       </c>
-      <c r="P10" s="5" t="str">
+      <c r="P10" s="6" t="str">
         <f t="shared" si="3"/>
         <v>0.857</v>
       </c>
-      <c r="Q10" s="5" t="str">
+      <c r="Q10" s="6" t="str">
         <f t="shared" si="4"/>
         <v>1.302</v>
       </c>
@@ -880,27 +880,27 @@
       <c r="L11" s="3">
         <v>0.0</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="5" t="str">
+      <c r="M11" s="5"/>
+      <c r="N11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>0.222</v>
       </c>
-      <c r="O11" s="5" t="str">
+      <c r="O11" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0.222</v>
       </c>
-      <c r="P11" s="5" t="str">
+      <c r="P11" s="6" t="str">
         <f t="shared" si="3"/>
         <v>0.222</v>
       </c>
-      <c r="Q11" s="5" t="str">
+      <c r="Q11" s="6" t="str">
         <f t="shared" si="4"/>
         <v>0.444</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="str">
         <f t="shared" ref="B12:C12" si="16">1</f>
@@ -939,27 +939,27 @@
       <c r="L12" s="3">
         <v>0.0</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="5" t="str">
+      <c r="M12" s="5"/>
+      <c r="N12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>1.000</v>
       </c>
-      <c r="O12" s="5" t="str">
+      <c r="O12" s="6" t="str">
         <f t="shared" si="2"/>
         <v>1.000</v>
       </c>
-      <c r="P12" s="5" t="str">
+      <c r="P12" s="6" t="str">
         <f t="shared" si="3"/>
         <v>1.000</v>
       </c>
-      <c r="Q12" s="5" t="str">
+      <c r="Q12" s="6" t="str">
         <f t="shared" si="4"/>
         <v>2.000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" ref="B13:L13" si="18">sum(B2:B12)</f>
@@ -1006,28 +1006,28 @@
         <v>3</v>
       </c>
       <c r="M13" s="3"/>
-      <c r="N13" s="6" t="str">
+      <c r="N13" s="7" t="str">
         <f t="shared" si="1"/>
         <v>0.533</v>
       </c>
-      <c r="O13" s="6" t="str">
+      <c r="O13" s="7" t="str">
         <f t="shared" si="2"/>
         <v>0.531</v>
       </c>
-      <c r="P13" s="6" t="str">
+      <c r="P13" s="7" t="str">
         <f t="shared" si="3"/>
         <v>0.663</v>
       </c>
-      <c r="Q13" s="6" t="str">
+      <c r="Q13" s="7" t="str">
         <f t="shared" si="4"/>
         <v>1.194</v>
       </c>
     </row>
     <row r="17">
-      <c r="N17" s="7"/>
+      <c r="N17" s="4"/>
     </row>
     <row r="18">
-      <c r="G18" s="7"/>
+      <c r="G18" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1105,45 +1105,49 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="R1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="3" t="str">
-        <f>4+4+3+5+3+5</f>
-        <v>24</v>
+        <f>4+4+3+5+3+5+5</f>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f>4+2+3+5+3+5</f>
-        <v>22</v>
+        <f>4+2+3+5+3+5+4</f>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>3+3+2+3+2+4</f>
+        <f>3+3+2+3+2+4+4</f>
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="str">
+        <f>4+2+2+4+2+4+3</f>
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f>2+1</f>
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="str">
+        <f t="shared" ref="G2:H2" si="1">1+1
+</f>
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>3+4+5+3+2
+</f>
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="str">
-        <f>4+2+2+4+2+4</f>
-        <v>18</v>
-      </c>
-      <c r="F2" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="H2" s="3" t="str">
-        <f>1+1
-</f>
-        <v>2</v>
-      </c>
-      <c r="I2" s="3" t="str">
-        <f>3+4+5+3
-</f>
-        <v>15</v>
-      </c>
-      <c r="J2" s="3">
-        <v>2.0</v>
+      <c r="J2" s="3" t="str">
+        <f>2+1</f>
+        <v>3</v>
       </c>
       <c r="K2" s="3">
         <v>0.0</v>
@@ -1151,22 +1155,22 @@
       <c r="L2" s="3">
         <v>0.0</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5" t="str">
-        <f t="shared" ref="N2:N17" si="1">IF(C2,E2/C2,)</f>
-        <v>0.818</v>
-      </c>
-      <c r="O2" s="5" t="str">
-        <f t="shared" ref="O2:O18" si="2">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
-        <v>0.833</v>
-      </c>
-      <c r="P2" s="5" t="str">
-        <f t="shared" ref="P2:P17" si="3">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
-        <v>1.273</v>
-      </c>
-      <c r="Q2" s="5" t="str">
-        <f t="shared" ref="Q2:Q18" si="4">IF(P2,P2+O2,)</f>
-        <v>2.106</v>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6" t="str">
+        <f t="shared" ref="N2:N17" si="2">IF(C2,E2/C2,)</f>
+        <v>0.808</v>
+      </c>
+      <c r="O2" s="6" t="str">
+        <f t="shared" ref="O2:O18" si="3">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
+        <v>0.828</v>
+      </c>
+      <c r="P2" s="6" t="str">
+        <f t="shared" ref="P2:P17" si="4">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
+        <v>1.308</v>
+      </c>
+      <c r="Q2" s="6" t="str">
+        <f t="shared" ref="Q2:Q18" si="5">IF(P2,P2+O2,)</f>
+        <v>2.135</v>
       </c>
     </row>
     <row r="3">
@@ -1174,25 +1178,25 @@
         <v>18</v>
       </c>
       <c r="B3" s="3" t="str">
-        <f>4+4+3+4+3+5</f>
-        <v>23</v>
+        <f>4+4+3+4+3+5+5</f>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f>4+4+3+3+2+5</f>
-        <v>21</v>
+        <f>4+4+3+3+2+5+5</f>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>3+3+1+1+2</f>
-        <v>10</v>
+        <f>3+3+1+1+2+4</f>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>3+3+1+2+4</f>
-        <v>13</v>
+        <f>3+3+1+2+4+4</f>
+        <v>17</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f>2+1
-</f>
-        <v>3</v>
+        <f>2+1+3
+</f>
+        <v>6</v>
       </c>
       <c r="G3" s="3">
         <v>1.0</v>
@@ -1202,8 +1206,8 @@
         <v>2</v>
       </c>
       <c r="I3" s="3" t="str">
-        <f>2+4+2+3</f>
-        <v>11</v>
+        <f>2+4+2+3+3</f>
+        <v>14</v>
       </c>
       <c r="J3" s="3" t="str">
         <f>1
@@ -1216,22 +1220,22 @@
       <c r="L3" s="3">
         <v>1.0</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.619</v>
-      </c>
-      <c r="O3" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.609</v>
-      </c>
-      <c r="P3" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>1.143</v>
-      </c>
-      <c r="Q3" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.752</v>
+      <c r="M3" s="5"/>
+      <c r="N3" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.654</v>
+      </c>
+      <c r="O3" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>0.643</v>
+      </c>
+      <c r="P3" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1.192</v>
+      </c>
+      <c r="Q3" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1.835</v>
       </c>
     </row>
     <row r="4">
@@ -1255,7 +1259,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f t="shared" ref="F4:F5" si="5">1+1
+        <f t="shared" ref="F4:F5" si="6">1+1
 </f>
         <v>2</v>
       </c>
@@ -1281,21 +1285,21 @@
 </f>
         <v>1</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="6" t="str">
+        <f t="shared" si="2"/>
         <v>0.778</v>
       </c>
-      <c r="O4" s="5" t="str">
-        <f t="shared" si="2"/>
+      <c r="O4" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>0.750</v>
       </c>
-      <c r="P4" s="5" t="str">
-        <f t="shared" si="3"/>
+      <c r="P4" s="6" t="str">
+        <f t="shared" si="4"/>
         <v>1.000</v>
       </c>
-      <c r="Q4" s="5" t="str">
-        <f t="shared" si="4"/>
+      <c r="Q4" s="6" t="str">
+        <f t="shared" si="5"/>
         <v>1.750</v>
       </c>
     </row>
@@ -1304,42 +1308,44 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="str">
-        <f>4+3+4+3+5</f>
-        <v>19</v>
+        <f>4+3+4+3+5+5</f>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="str">
-        <f>4+3+3+3+5
-</f>
-        <v>18</v>
+        <f>4+3+3+3+5+4
+</f>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>1+1+3+3</f>
-        <v>8</v>
+        <f>1+1+3+3+3</f>
+        <v>11</v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>3+2+3+4
-</f>
-        <v>12</v>
+        <f>3+2+3+4+3
+</f>
+        <v>15</v>
       </c>
       <c r="F5" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G5" s="3" t="str">
-        <f>3+1
-</f>
-        <v>4</v>
+        <f>3+1+2
+</f>
+        <v>6</v>
       </c>
       <c r="H5" s="3">
         <v>1.0</v>
       </c>
       <c r="I5" s="3" t="str">
-        <f>5+4+4
-</f>
-        <v>13</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.0</v>
+        <f>5+4+4+3
+</f>
+        <v>16</v>
+      </c>
+      <c r="J5" s="3" t="str">
+        <f>1
+</f>
+        <v>1</v>
       </c>
       <c r="K5" s="3">
         <v>1.0</v>
@@ -1347,22 +1353,22 @@
       <c r="L5" s="3">
         <v>1.0</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.682</v>
+      </c>
+      <c r="O5" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>0.667</v>
       </c>
-      <c r="O5" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.632</v>
-      </c>
-      <c r="P5" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>1.389</v>
-      </c>
-      <c r="Q5" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>2.020</v>
+      <c r="P5" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1.455</v>
+      </c>
+      <c r="Q5" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>2.121</v>
       </c>
     </row>
     <row r="6">
@@ -1410,21 +1416,21 @@
       <c r="L6" s="3">
         <v>0.0</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6" t="str">
+        <f t="shared" si="2"/>
         <v>0.556</v>
       </c>
-      <c r="O6" s="5" t="str">
-        <f t="shared" si="2"/>
+      <c r="O6" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>0.600</v>
       </c>
-      <c r="P6" s="5" t="str">
-        <f t="shared" si="3"/>
+      <c r="P6" s="6" t="str">
+        <f t="shared" si="4"/>
         <v>0.556</v>
       </c>
-      <c r="Q6" s="5" t="str">
-        <f t="shared" si="4"/>
+      <c r="Q6" s="6" t="str">
+        <f t="shared" si="5"/>
         <v>1.156</v>
       </c>
     </row>
@@ -1433,32 +1439,32 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="str">
-        <f>4+3+4+3+5</f>
-        <v>19</v>
+        <f>4+3+4+3+5+5</f>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f>4+3+4+3+4</f>
-        <v>18</v>
+        <f>4+3+4+3+4+5</f>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>1+3+1+1
-</f>
-        <v>6</v>
+        <f>1+3+1+1+3
+</f>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>3+2+3+2+3
-</f>
-        <v>13</v>
+        <f>3+2+3+2+3+4
+</f>
+        <v>17</v>
       </c>
       <c r="F7" s="3" t="str">
-        <f>1+2
+        <f>1+2+2
+</f>
+        <v>5</v>
+      </c>
+      <c r="G7" s="3" t="str">
+        <f>1+1+1
 </f>
         <v>3</v>
-      </c>
-      <c r="G7" s="3" t="str">
-        <f>1+1
-</f>
-        <v>2</v>
       </c>
       <c r="H7" s="3" t="str">
         <f>1
@@ -1466,8 +1472,8 @@
         <v>1</v>
       </c>
       <c r="I7" s="3" t="str">
-        <f>1+1+2+1+2</f>
-        <v>7</v>
+        <f>1+1+2+1+2+5</f>
+        <v>12</v>
       </c>
       <c r="J7" s="3">
         <v>0.0</v>
@@ -1476,49 +1482,49 @@
         <v>0.0</v>
       </c>
       <c r="L7" s="3" t="str">
-        <f>1
-</f>
-        <v>1</v>
-      </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.722</v>
-      </c>
-      <c r="O7" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.684</v>
-      </c>
-      <c r="P7" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>1.278</v>
-      </c>
-      <c r="Q7" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.962</v>
+        <f t="shared" ref="L7:L8" si="7">1
+</f>
+        <v>1</v>
+      </c>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.739</v>
+      </c>
+      <c r="O7" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>0.708</v>
+      </c>
+      <c r="P7" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1.348</v>
+      </c>
+      <c r="Q7" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>2.056</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="str">
-        <f t="shared" ref="B8:C8" si="6">4+3+3+4+2+5</f>
-        <v>21</v>
+        <f>4+3+3+4+2+5+5</f>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v>21</v>
+        <f>4+3+3+4+2+5+2</f>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="str">
-        <f>2+1+1
-</f>
-        <v>4</v>
+        <f>2+1+1+2
+</f>
+        <v>6</v>
       </c>
       <c r="E8" s="3" t="str">
-        <f>9+2+1+2
-</f>
-        <v>14</v>
+        <f>9+2+1+2+2
+</f>
+        <v>16</v>
       </c>
       <c r="F8" s="3">
         <v>2.0</v>
@@ -1530,34 +1536,36 @@
         <v>0.0</v>
       </c>
       <c r="I8" s="3" t="str">
-        <f>3+1+3+1+3</f>
-        <v>11</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.0</v>
+        <f>3+1+3+1+3+3</f>
+        <v>14</v>
+      </c>
+      <c r="J8" s="3" t="str">
+        <f>2</f>
+        <v>2</v>
       </c>
       <c r="K8" s="3">
         <v>0.0</v>
       </c>
-      <c r="L8" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.667</v>
-      </c>
-      <c r="O8" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.667</v>
-      </c>
-      <c r="P8" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.857</v>
-      </c>
-      <c r="Q8" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.524</v>
+      <c r="L8" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.696</v>
+      </c>
+      <c r="O8" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>0.692</v>
+      </c>
+      <c r="P8" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0.870</v>
+      </c>
+      <c r="Q8" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1.562</v>
       </c>
     </row>
     <row r="9">
@@ -1596,7 +1604,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="3" t="str">
-        <f>1
+        <f t="shared" ref="J9:J13" si="8">1
 </f>
         <v>1</v>
       </c>
@@ -1606,21 +1614,21 @@
       <c r="L9" s="3">
         <v>0.0</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="6" t="str">
+        <f t="shared" si="2"/>
         <v>0.625</v>
       </c>
-      <c r="O9" s="5" t="str">
-        <f t="shared" si="2"/>
+      <c r="O9" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>0.667</v>
       </c>
-      <c r="P9" s="5" t="str">
-        <f t="shared" si="3"/>
+      <c r="P9" s="6" t="str">
+        <f t="shared" si="4"/>
         <v>0.625</v>
       </c>
-      <c r="Q9" s="5" t="str">
-        <f t="shared" si="4"/>
+      <c r="Q9" s="6" t="str">
+        <f t="shared" si="5"/>
         <v>1.292</v>
       </c>
     </row>
@@ -1629,20 +1637,20 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="str">
-        <f t="shared" ref="B10:C10" si="7">4+4+3+2+5</f>
-        <v>18</v>
+        <f>4+4+3+2+5+5</f>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>18</v>
+        <f>4+4+3+2+5+4</f>
+        <v>22</v>
       </c>
       <c r="D10" s="3" t="str">
-        <f>1+2+1+1</f>
-        <v>5</v>
+        <f>1+2+1+1+2</f>
+        <v>7</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f>2+2+2+1+2</f>
-        <v>9</v>
+        <f>2+2+2+1+2+3</f>
+        <v>12</v>
       </c>
       <c r="F10" s="3">
         <v>0.0</v>
@@ -1654,11 +1662,12 @@
         <v>0.0</v>
       </c>
       <c r="I10" s="3" t="str">
-        <f>1+1+1+1</f>
-        <v>4</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0.0</v>
+        <f>1+1+1+1+2</f>
+        <v>6</v>
+      </c>
+      <c r="J10" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="K10" s="3">
         <v>0.0</v>
@@ -1666,22 +1675,22 @@
       <c r="L10" s="3">
         <v>0.0</v>
       </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.500</v>
-      </c>
-      <c r="O10" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.500</v>
-      </c>
-      <c r="P10" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.500</v>
-      </c>
-      <c r="Q10" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.000</v>
+      <c r="M10" s="5"/>
+      <c r="N10" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.545</v>
+      </c>
+      <c r="O10" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>0.565</v>
+      </c>
+      <c r="P10" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0.545</v>
+      </c>
+      <c r="Q10" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1.111</v>
       </c>
     </row>
     <row r="11">
@@ -1689,21 +1698,21 @@
         <v>24</v>
       </c>
       <c r="B11" s="3" t="str">
-        <f t="shared" ref="B11:C11" si="8">3+3+3+4+2</f>
-        <v>15</v>
+        <f>3+3+3+4+2+5</f>
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>15</v>
+        <f>3+3+3+4+2+4</f>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="str">
-        <f>2+1+1+4</f>
-        <v>8</v>
+        <f>2+1+1+4+3</f>
+        <v>11</v>
       </c>
       <c r="E11" s="3" t="str">
-        <f>2+2+4+1
-</f>
-        <v>9</v>
+        <f>2+2+4+1+4
+</f>
+        <v>13</v>
       </c>
       <c r="F11" s="3" t="str">
         <f>1+1
@@ -1720,8 +1729,9 @@
         <f>2+1+1+3</f>
         <v>7</v>
       </c>
-      <c r="J11" s="3">
-        <v>0.0</v>
+      <c r="J11" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="K11" s="3">
         <v>0.0</v>
@@ -1729,44 +1739,44 @@
       <c r="L11" s="3">
         <v>0.0</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.600</v>
-      </c>
-      <c r="O11" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.600</v>
-      </c>
-      <c r="P11" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.867</v>
-      </c>
-      <c r="Q11" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.467</v>
+      <c r="M11" s="5"/>
+      <c r="N11" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.684</v>
+      </c>
+      <c r="O11" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>0.700</v>
+      </c>
+      <c r="P11" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0.895</v>
+      </c>
+      <c r="Q11" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1.595</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="str">
-        <f t="shared" ref="B12:C12" si="9">3+3+3+4+4</f>
-        <v>17</v>
+        <f>3+3+3+4+4+4</f>
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v>17</v>
+        <f>3+3+3+4+4+3</f>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="str">
-        <f>1+2+3
-</f>
-        <v>6</v>
+        <f>1+2+3+2
+</f>
+        <v>8</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f>1+1+1+3+3</f>
-        <v>9</v>
+        <f>1+1+1+3+3+2</f>
+        <v>11</v>
       </c>
       <c r="F12" s="3">
         <v>1.0</v>
@@ -1780,11 +1790,12 @@
         <v>1</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f>1+1+2+1</f>
-        <v>5</v>
-      </c>
-      <c r="J12" s="3">
-        <v>0.0</v>
+        <f>1+1+2+1+1</f>
+        <v>6</v>
+      </c>
+      <c r="J12" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="K12" s="3">
         <v>0.0</v>
@@ -1792,22 +1803,22 @@
       <c r="L12" s="3">
         <v>0.0</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.529</v>
-      </c>
-      <c r="O12" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.529</v>
-      </c>
-      <c r="P12" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.765</v>
-      </c>
-      <c r="Q12" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.294</v>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.550</v>
+      </c>
+      <c r="O12" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>0.571</v>
+      </c>
+      <c r="P12" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0.750</v>
+      </c>
+      <c r="Q12" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1.321</v>
       </c>
     </row>
     <row r="13">
@@ -1815,24 +1826,26 @@
         <v>25</v>
       </c>
       <c r="B13" s="3" t="str">
-        <f t="shared" ref="B13:B14" si="10">3+3+3+4+2+4</f>
-        <v>19</v>
+        <f t="shared" ref="B13:B14" si="9">3+3+3+4+2+4+4</f>
+        <v>23</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f>3+3+3+4+1+4</f>
-        <v>18</v>
+        <f>3+3+3+4+1+4+4</f>
+        <v>22</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f>2+1+3+2+1
-</f>
-        <v>9</v>
+        <f>2+1+3+2+1+2
+</f>
+        <v>11</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f>2+2+1+3+2</f>
-        <v>10</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1.0</v>
+        <f>2+2+1+3+2+2</f>
+        <v>12</v>
+      </c>
+      <c r="F13" s="3" t="str">
+        <f>1+1
+</f>
+        <v>2</v>
       </c>
       <c r="G13" s="3">
         <v>0.0</v>
@@ -1841,13 +1854,12 @@
         <v>0.0</v>
       </c>
       <c r="I13" s="3" t="str">
-        <f>2+3+1
-</f>
-        <v>6</v>
+        <f>2+3+1+5
+</f>
+        <v>11</v>
       </c>
       <c r="J13" s="3" t="str">
-        <f>1
-</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="K13" s="3">
@@ -1856,22 +1868,22 @@
       <c r="L13" s="3">
         <v>0.0</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.556</v>
-      </c>
-      <c r="O13" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.579</v>
-      </c>
-      <c r="P13" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.611</v>
-      </c>
-      <c r="Q13" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.190</v>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.545</v>
+      </c>
+      <c r="O13" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>0.565</v>
+      </c>
+      <c r="P13" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0.636</v>
+      </c>
+      <c r="Q13" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1.202</v>
       </c>
     </row>
     <row r="14">
@@ -1879,20 +1891,20 @@
         <v>27</v>
       </c>
       <c r="B14" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>19</v>
+        <f t="shared" si="9"/>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="str">
-        <f>3+3+3+4+1+3</f>
-        <v>17</v>
+        <f>3+3+3+4+1+3+4</f>
+        <v>21</v>
       </c>
       <c r="D14" s="3" t="str">
-        <f>1+1+3+2+3</f>
-        <v>10</v>
+        <f>1+1+3+2+3+1</f>
+        <v>11</v>
       </c>
       <c r="E14" s="3" t="str">
-        <f>1+2+1+3+2</f>
-        <v>9</v>
+        <f>1+2+1+3+2+2</f>
+        <v>11</v>
       </c>
       <c r="F14" s="3">
         <v>0.0</v>
@@ -1904,9 +1916,9 @@
         <v>0.0</v>
       </c>
       <c r="I14" s="3" t="str">
-        <f>1+3+1
-</f>
-        <v>5</v>
+        <f>1+3+1+2
+</f>
+        <v>7</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>1+1
@@ -1919,22 +1931,22 @@
       <c r="L14" s="3">
         <v>0.0</v>
       </c>
-      <c r="M14" s="4"/>
-      <c r="N14" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.529</v>
-      </c>
-      <c r="O14" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.579</v>
-      </c>
-      <c r="P14" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.529</v>
-      </c>
-      <c r="Q14" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.108</v>
+      <c r="M14" s="5"/>
+      <c r="N14" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.524</v>
+      </c>
+      <c r="O14" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>0.565</v>
+      </c>
+      <c r="P14" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0.524</v>
+      </c>
+      <c r="Q14" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1.089</v>
       </c>
     </row>
     <row r="15">
@@ -1942,12 +1954,12 @@
         <v>31</v>
       </c>
       <c r="B15" s="3" t="str">
-        <f t="shared" ref="B15:C15" si="11">3+4
+        <f t="shared" ref="B15:C15" si="10">3+4
 </f>
         <v>7</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="D15" s="3">
@@ -1979,21 +1991,21 @@
       <c r="L15" s="3">
         <v>0.0</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6" t="str">
+        <f t="shared" si="2"/>
         <v>0.571</v>
       </c>
-      <c r="O15" s="5" t="str">
-        <f t="shared" si="2"/>
+      <c r="O15" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>0.571</v>
       </c>
-      <c r="P15" s="5" t="str">
-        <f t="shared" si="3"/>
+      <c r="P15" s="6" t="str">
+        <f t="shared" si="4"/>
         <v>0.571</v>
       </c>
-      <c r="Q15" s="5" t="str">
-        <f t="shared" si="4"/>
+      <c r="Q15" s="6" t="str">
+        <f t="shared" si="5"/>
         <v>1.143</v>
       </c>
     </row>
@@ -2034,21 +2046,21 @@
       <c r="L16" s="3">
         <v>0.0</v>
       </c>
-      <c r="M16" s="4"/>
-      <c r="N16" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="6" t="str">
+        <f t="shared" si="2"/>
         <v>1.000</v>
       </c>
-      <c r="O16" s="5" t="str">
-        <f t="shared" si="2"/>
+      <c r="O16" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>1.000</v>
       </c>
-      <c r="P16" s="5" t="str">
-        <f t="shared" si="3"/>
+      <c r="P16" s="6" t="str">
+        <f t="shared" si="4"/>
         <v>1.667</v>
       </c>
-      <c r="Q16" s="5" t="str">
-        <f t="shared" si="4"/>
+      <c r="Q16" s="6" t="str">
+        <f t="shared" si="5"/>
         <v>2.667</v>
       </c>
     </row>
@@ -2089,95 +2101,95 @@
       <c r="L17" s="3">
         <v>0.0</v>
       </c>
-      <c r="M17" s="4"/>
-      <c r="N17" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="6" t="str">
+        <f t="shared" si="2"/>
         <v>0.333</v>
       </c>
-      <c r="O17" s="5" t="str">
-        <f t="shared" si="2"/>
+      <c r="O17" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>0.500</v>
       </c>
-      <c r="P17" s="5" t="str">
-        <f t="shared" si="3"/>
+      <c r="P17" s="6" t="str">
+        <f t="shared" si="4"/>
         <v>0.333</v>
       </c>
-      <c r="Q17" s="5" t="str">
-        <f t="shared" si="4"/>
+      <c r="Q17" s="6" t="str">
+        <f t="shared" si="5"/>
         <v>0.833</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f t="shared" ref="B18:L18" si="12">sum(B2:B17)</f>
-        <v>239</v>
+        <f t="shared" ref="B18:L18" si="11">sum(B2:B17)</f>
+        <v>286</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>224</v>
+        <f t="shared" si="11"/>
+        <v>263</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>101</v>
+        <f t="shared" si="11"/>
+        <v>127</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>141</v>
+        <f t="shared" si="11"/>
+        <v>170</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>20</v>
+        <f t="shared" si="11"/>
+        <v>27</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>10</v>
+        <f t="shared" si="11"/>
+        <v>14</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>101</v>
+        <f t="shared" si="11"/>
+        <v>127</v>
       </c>
       <c r="J18" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>11</v>
+        <f t="shared" si="11"/>
+        <v>18</v>
       </c>
       <c r="K18" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="L18" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="11"/>
+        <v>5</v>
       </c>
       <c r="M18" s="3"/>
-      <c r="N18" s="6" t="str">
+      <c r="N18" s="7" t="str">
         <f>E18/C18</f>
-        <v>0.629</v>
-      </c>
-      <c r="O18" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>0.636</v>
-      </c>
-      <c r="P18" s="6" t="str">
+        <v>0.646</v>
+      </c>
+      <c r="O18" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>0.657</v>
+      </c>
+      <c r="P18" s="7" t="str">
         <f>((E18-F18-G18-H18)+(2*F18)+(3*G18)+(4*H18))/C18</f>
-        <v>0.902</v>
-      </c>
-      <c r="Q18" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>1.538</v>
+        <v>0.935</v>
+      </c>
+      <c r="Q18" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>1.593</v>
       </c>
     </row>
     <row r="22">
-      <c r="N22" s="7"/>
+      <c r="N22" s="4"/>
     </row>
     <row r="23">
-      <c r="G23" s="7"/>
+      <c r="G23" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Name games as 'Season Year MM/DD'
</commit_message>
<xml_diff>
--- a/Minor League Scientists Stats.xlsx
+++ b/Minor League Scientists Stats.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Fall 2015 09.09.15" sheetId="1" r:id="rId1"/>
-    <sheet name="Fall 2015 09.16.15" sheetId="3" r:id="rId2"/>
+    <sheet name="Fall 2015 09.09" sheetId="1" r:id="rId1"/>
+    <sheet name="Fall 2015 09.16" sheetId="3" r:id="rId2"/>
     <sheet name="Tournament Fall 2015" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -1640,7 +1640,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Add Joe Perryman's last name
</commit_message>
<xml_diff>
--- a/Minor League Scientists Stats.xlsx
+++ b/Minor League Scientists Stats.xlsx
@@ -120,19 +120,28 @@
     <t>Amory Meltzer</t>
   </si>
   <si>
-    <t>Joe P</t>
+    <t>Nick Hanten</t>
+  </si>
+  <si>
+    <t>Sean Aronow</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Joe Perryman</t>
   </si>
   <si>
     <t>Jeremy Lindsey</t>
   </si>
   <si>
-    <t>Total:</t>
+    <t>Jake Galbraith</t>
   </si>
   <si>
-    <t>Nick Hanten</t>
+    <t>Morgan Dunkin</t>
   </si>
   <si>
-    <t>Sean Aronow</t>
+    <t>Oliver Patton</t>
   </si>
   <si>
     <t>Nick Mirman</t>
@@ -141,19 +150,10 @@
     <t>Scott Richardson</t>
   </si>
   <si>
-    <t>Oliver Patton</t>
-  </si>
-  <si>
     <t>Alex Potter</t>
   </si>
   <si>
     <t>Jackson Badger</t>
-  </si>
-  <si>
-    <t>Jake Galbraith</t>
-  </si>
-  <si>
-    <t>Morgan Dunkin</t>
   </si>
   <si>
     <t>Matt Turner</t>
@@ -888,7 +888,7 @@
     </row>
     <row r="11" ht="15.0" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2">
         <v>2.0</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2">
         <v>2.0</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>2.0</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2">
         <v>3.0</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>4.0</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>3.0</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2">
         <v>3.0</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>4.0</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>4.0</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>3.0</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2">
         <v>2.0</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>4.0</v>
@@ -3123,7 +3123,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2">
         <v>2.0</v>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2">
         <v>3.0</v>
@@ -3542,7 +3542,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>3.0</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2">
         <v>3.0</v>
@@ -3682,7 +3682,7 @@
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2">
         <v>3.0</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="2" ht="15.0" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2">
         <v>3.0</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2">
         <v>3.0</v>
@@ -4066,7 +4066,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>2.0</v>
@@ -4240,7 +4240,7 @@
     </row>
     <row r="2" ht="15.0" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2">
         <v>4.0</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2">
         <v>4.0</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>2.0</v>
@@ -4694,7 +4694,7 @@
     </row>
     <row r="3" ht="15.0" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2">
         <v>4.0</v>
@@ -4904,7 +4904,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>3.0</v>
@@ -5288,7 +5288,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2">
         <v>3.0</v>
@@ -5323,7 +5323,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>3.0</v>
@@ -5358,7 +5358,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>3.0</v>
@@ -5777,7 +5777,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>3.0</v>
@@ -5917,7 +5917,7 @@
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2">
         <v>4.0</v>
@@ -6161,7 +6161,7 @@
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2">
         <v>4.0</v>
@@ -6196,7 +6196,7 @@
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
         <v>3.0</v>
@@ -6231,7 +6231,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>4.0</v>
@@ -6545,7 +6545,7 @@
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2">
         <v>4.0</v>
@@ -6580,7 +6580,7 @@
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
         <v>3.0</v>
@@ -6650,7 +6650,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>4.0</v>
@@ -6964,7 +6964,7 @@
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2">
         <v>4.0</v>
@@ -6999,7 +6999,7 @@
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
         <v>3.0</v>
@@ -7453,7 +7453,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2">
         <v>3.0</v>
@@ -7488,7 +7488,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>3.0</v>
@@ -8151,7 +8151,7 @@
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2">
         <v>4.0</v>
@@ -8570,7 +8570,7 @@
     </row>
     <row r="3" ht="15.0" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2">
         <v>2.0</v>
@@ -9199,7 +9199,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2">
         <v>2.0</v>
@@ -9688,7 +9688,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2">
         <v>4.0</v>
@@ -9758,7 +9758,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2">
         <v>3.0</v>
@@ -10177,7 +10177,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2">
         <v>3.0</v>
@@ -10352,7 +10352,7 @@
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2">
         <v>3.0</v>
@@ -10806,7 +10806,7 @@
     </row>
     <row r="11" ht="15.0" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <v>3.0</v>
@@ -11120,7 +11120,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>4.0</v>
@@ -11574,7 +11574,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4">
         <v>4.0</v>
@@ -11609,7 +11609,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4">
         <v>4.0</v>
@@ -11993,7 +11993,7 @@
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4">
         <v>5.0</v>
@@ -12028,7 +12028,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4">
         <v>5.0</v>
@@ -12482,7 +12482,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4">
         <v>2.0</v>
@@ -12517,7 +12517,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4">
         <v>2.0</v>
@@ -12971,7 +12971,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4">
         <v>3.0</v>
@@ -13041,7 +13041,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4">
         <v>3.0</v>
@@ -13390,7 +13390,7 @@
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4">
         <v>2.0</v>
@@ -13460,7 +13460,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4">
         <v>3.0</v>
@@ -13495,7 +13495,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4">
         <v>3.0</v>
@@ -13879,7 +13879,7 @@
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4">
         <v>3.0</v>
@@ -13914,7 +13914,7 @@
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4">
         <v>4.0</v>
@@ -14019,7 +14019,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4">
         <v>4.0</v>
@@ -14438,7 +14438,7 @@
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4">
         <v>5.0</v>
@@ -14473,7 +14473,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4">
         <v>3.0</v>
@@ -14508,7 +14508,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4">
         <v>3.0</v>
@@ -14891,7 +14891,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4">
         <v>3.0</v>
@@ -14926,7 +14926,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4">
         <v>2.0</v>
@@ -14996,7 +14996,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4">
         <v>4.0</v>
@@ -15379,7 +15379,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6">
         <v>3.0</v>
@@ -15838,7 +15838,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2">
         <v>3.0</v>
@@ -15873,7 +15873,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2">
         <v>3.0</v>
@@ -15908,7 +15908,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2">
         <v>3.0</v>
@@ -16256,7 +16256,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="6">
         <v>2.0</v>
@@ -16326,7 +16326,7 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6">
         <v>2.0</v>
@@ -16361,7 +16361,7 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6">
         <v>2.0</v>
@@ -16784,7 +16784,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6">
         <v>4.0</v>
@@ -16854,7 +16854,7 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="6">
         <v>3.0</v>
@@ -17277,7 +17277,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6">
         <v>5.0</v>
@@ -17312,7 +17312,7 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="6">
         <v>4.0</v>
@@ -17770,7 +17770,7 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="6">
         <v>1.0</v>
@@ -17805,7 +17805,7 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6">
         <v>2.0</v>
@@ -18263,7 +18263,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="6">
         <v>4.0</v>
@@ -18333,7 +18333,7 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="6">
         <v>4.0</v>
@@ -18791,7 +18791,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="6">
         <v>3.0</v>
@@ -18826,7 +18826,7 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="6">
         <v>3.0</v>
@@ -18896,7 +18896,7 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6">
         <v>3.0</v>
@@ -19284,7 +19284,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6">
         <v>4.0</v>
@@ -19354,7 +19354,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6">
         <v>3.0</v>
@@ -19812,7 +19812,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6">
         <v>4.0</v>
@@ -19882,7 +19882,7 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="6">
         <v>3.0</v>
@@ -20136,7 +20136,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6">
         <f>3+2+3</f>
@@ -20257,7 +20257,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" s="6">
         <f>3+3+4</f>
@@ -20491,7 +20491,7 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B12" s="6">
         <f>1</f>
@@ -20808,7 +20808,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>4.0</v>
@@ -20913,7 +20913,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>4.0</v>
@@ -21227,7 +21227,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>3.0</v>
@@ -21332,7 +21332,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>3.0</v>
@@ -21716,7 +21716,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2">
         <v>2.0</v>
@@ -21786,7 +21786,7 @@
     </row>
     <row r="11" ht="15.0" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2">
         <v>3.0</v>
@@ -21821,7 +21821,7 @@
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2">
         <v>3.0</v>
@@ -22135,7 +22135,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>4.0</v>
@@ -22205,7 +22205,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>2.0</v>
@@ -22275,7 +22275,7 @@
     </row>
     <row r="11" ht="15.0" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2">
         <v>3.0</v>
@@ -22554,7 +22554,7 @@
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
         <v>2.0</v>
@@ -22589,7 +22589,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2">
         <v>2.0</v>
@@ -22659,7 +22659,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>3.0</v>

</xml_diff>